<commit_message>
tidied up teh code, added functionality, continued with analyses
</commit_message>
<xml_diff>
--- a/data/Matrix_EOL_PD_.xlsx
+++ b/data/Matrix_EOL_PD_.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="explanatios" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="explanations" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="ledd" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="working" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="279">
   <si>
     <t xml:space="preserve">subj</t>
   </si>
@@ -550,6 +550,9 @@
     <t xml:space="preserve">dbs</t>
   </si>
   <si>
+    <t xml:space="preserve">Factor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unit</t>
   </si>
   <si>
@@ -975,15 +978,15 @@
   </sheetPr>
   <dimension ref="A1:FS297"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="FG1" activeCellId="0" sqref="FG1"/>
+      <selection pane="bottomRight" activeCell="V1" activeCellId="0" sqref="V1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="3.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.67"/>
@@ -1001,7 +1004,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="47" style="0" width="3.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="3.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="154" min="50" style="0" width="3.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="155" min="155" style="0" width="5.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="155" min="155" style="0" width="5.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="162" min="156" style="0" width="3.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="163" min="163" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="171" min="164" style="0" width="3.67"/>
@@ -52674,18 +52677,23 @@
   </sheetPr>
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.65625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="31.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="31.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>175</v>
+      </c>
       <c r="B1" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C1" s="0" t="n">
         <v>0</v>
@@ -52729,13 +52737,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52743,16 +52751,16 @@
         <v>3</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52760,7 +52768,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52768,7 +52776,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52776,7 +52784,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52784,43 +52792,43 @@
         <v>9</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52828,25 +52836,25 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52854,34 +52862,34 @@
         <v>11</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52889,22 +52897,22 @@
         <v>12</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52912,7 +52920,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52920,22 +52928,22 @@
         <v>14</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52943,19 +52951,19 @@
         <v>15</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52963,25 +52971,25 @@
         <v>16</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52989,22 +52997,22 @@
         <v>17</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53012,16 +53020,16 @@
         <v>18</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53029,16 +53037,16 @@
         <v>19</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53046,13 +53054,13 @@
         <v>20</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53060,13 +53068,13 @@
         <v>21</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53074,13 +53082,13 @@
         <v>22</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53088,19 +53096,19 @@
         <v>23</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53108,22 +53116,22 @@
         <v>24</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53131,28 +53139,28 @@
         <v>25</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53160,22 +53168,22 @@
         <v>26</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53183,28 +53191,28 @@
         <v>27</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53212,28 +53220,28 @@
         <v>28</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53241,31 +53249,31 @@
         <v>29</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53273,16 +53281,16 @@
         <v>30</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53290,16 +53298,16 @@
         <v>31</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53307,16 +53315,16 @@
         <v>32</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53324,16 +53332,16 @@
         <v>33</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53341,7 +53349,7 @@
         <v>50</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>0</v>
@@ -53370,73 +53378,73 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>0</v>
@@ -53453,10 +53461,10 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>0</v>
@@ -53485,25 +53493,25 @@
         <v>173</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53511,13 +53519,13 @@
         <v>174</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -53542,14 +53550,14 @@
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.65625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53666,7 +53674,7 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B16" s="3" t="n">
         <v>0.33</v>
@@ -53694,7 +53702,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="str">

</xml_diff>